<commit_message>
fixed smoother stemmer comvination
</commit_message>
<xml_diff>
--- a/test_result_comparison.xlsx
+++ b/test_result_comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\KULIAH\NLP\ws 1\postag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7818FBD8-0AD7-4ED9-89AE-9DCCBFE22611}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B87F472-2B58-4ED8-8848-FB371AD6C655}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{7137D254-8446-492D-A36E-CB983406DD6C}"/>
   </bookViews>
@@ -168,7 +168,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -251,21 +251,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -285,11 +270,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -321,19 +326,40 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -650,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CD14569-BAA4-4BB5-9D07-C84D0FF9988D}">
-  <dimension ref="B1:E37"/>
+  <dimension ref="B1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -676,7 +702,7 @@
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="15">
+      <c r="B2" s="17">
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -688,7 +714,7 @@
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="11" t="s">
         <v>15</v>
       </c>
@@ -698,7 +724,7 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="15"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="12" t="s">
         <v>16</v>
       </c>
@@ -708,288 +734,473 @@
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="13">
+      <c r="B5" s="18"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="18"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="19"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="20">
         <v>2</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="13"/>
-      <c r="C6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="13"/>
-      <c r="C7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="13">
-        <v>3</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>6</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="13"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="13"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="13">
-        <v>4</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
-      <c r="C12" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="13"/>
-      <c r="C13" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="B13" s="22"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="13">
-        <v>5</v>
+      <c r="B14" s="20">
+        <v>3</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="13"/>
-      <c r="C15" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="B15" s="21"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="13"/>
-      <c r="C16" s="7" t="s">
-        <v>20</v>
+      <c r="B16" s="21"/>
+      <c r="C16" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="13">
-        <v>6</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>9</v>
+      <c r="B17" s="21"/>
+      <c r="C17" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="13"/>
-      <c r="C18" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="B18" s="21"/>
+      <c r="C18" s="15"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="13"/>
-      <c r="C19" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="15"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="13">
-        <v>7</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="B20" s="22"/>
+      <c r="C20" s="15"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="13"/>
-      <c r="C21" s="6" t="s">
-        <v>15</v>
+      <c r="B21" s="20">
+        <v>4</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="13"/>
-      <c r="C22" s="7" t="s">
-        <v>22</v>
+      <c r="B22" s="21"/>
+      <c r="C22" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="13">
-        <v>8</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>11</v>
+      <c r="B23" s="21"/>
+      <c r="C23" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="13"/>
-      <c r="C24" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="15"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="13"/>
-      <c r="C25" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="13">
-        <v>9</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="B26" s="22"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="13"/>
-      <c r="C27" s="6" t="s">
-        <v>15</v>
+      <c r="B27" s="20">
+        <v>5</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="13"/>
-      <c r="C28" s="7" t="s">
-        <v>24</v>
+      <c r="B28" s="21"/>
+      <c r="C28" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="13">
-        <v>10</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>13</v>
+      <c r="B29" s="21"/>
+      <c r="C29" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B30" s="13"/>
-      <c r="C30" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="15"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="13"/>
-      <c r="C31" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="15"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="13">
-        <v>11</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="B32" s="22"/>
+      <c r="C32" s="15"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="13"/>
-      <c r="C33" s="6" t="s">
-        <v>15</v>
+      <c r="B33" s="20">
+        <v>6</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="13"/>
-      <c r="C34" s="7" t="s">
-        <v>26</v>
+      <c r="B34" s="21"/>
+      <c r="C34" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="14"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="14"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B37" s="14"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B38" s="22"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39" s="20">
+        <v>7</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40" s="21"/>
+      <c r="C40" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B41" s="21"/>
+      <c r="C41" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42" s="21"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B43" s="21"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B44" s="22"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B45" s="20">
+        <v>8</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B46" s="21"/>
+      <c r="C46" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B47" s="21"/>
+      <c r="C47" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B48" s="21"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B49" s="21"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B50" s="22"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B51" s="20">
+        <v>9</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B52" s="21"/>
+      <c r="C52" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B53" s="21"/>
+      <c r="C53" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B54" s="21"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B55" s="21"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B56" s="22"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B57" s="20">
+        <v>10</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B58" s="21"/>
+      <c r="C58" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B59" s="21"/>
+      <c r="C59" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B60" s="21"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B61" s="21"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B62" s="22"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B63" s="13">
+        <v>11</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B64" s="13"/>
+      <c r="C64" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B65" s="13"/>
+      <c r="C65" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B66" s="13"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B67" s="13"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B68" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B32:B34"/>
+  <mergeCells count="11">
+    <mergeCell ref="B57:B62"/>
+    <mergeCell ref="B63:B68"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="B39:B44"/>
+    <mergeCell ref="B45:B50"/>
+    <mergeCell ref="B51:B56"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="B21:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed some more stem smooth bug
</commit_message>
<xml_diff>
--- a/test_result_comparison.xlsx
+++ b/test_result_comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\KULIAH\NLP\ws 1\postag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B87F472-2B58-4ED8-8848-FB371AD6C655}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B694974-A467-4CCA-87BB-67586114B1C2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{7137D254-8446-492D-A36E-CB983406DD6C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Kalimat</t>
   </si>
@@ -54,9 +54,6 @@
     <t xml:space="preserve">RB VB CD NND IN NNP IN VB VB NN SC NN PR Z SC SC RP PRP VB NN PR SC RB VB IN NN IN NN NNP Z </t>
   </si>
   <si>
-    <t xml:space="preserve">NNP PR ADV VB IN NNP Z SC X in NNP NEG JJ SC NN RP Z </t>
-  </si>
-  <si>
     <t xml:space="preserve">CD NN NNP VB NNP Z JJ SC CD IN CD NN NNP JJ Z </t>
   </si>
   <si>
@@ -127,6 +124,42 @@
   </si>
   <si>
     <t>Legend</t>
+  </si>
+  <si>
+    <t>Model smooth dan stem</t>
+  </si>
+  <si>
+    <t>NND NN SC VB NN NN JJ Z RB JJ Z CC VB NN VB JJ Z</t>
+  </si>
+  <si>
+    <t>CD NND NN NN PR MD VB VB CD NN SC RB JJ IN NNP SC VB NN JJ PRP Z</t>
+  </si>
+  <si>
+    <t>NN PR RB VB IN NNP Z SC VB IN NNP NEG VB SC VB PRP Z</t>
+  </si>
+  <si>
+    <t>NN NNP NNP VB NNP Z VB IN CD IN CD NN NNP JJ Z</t>
+  </si>
+  <si>
+    <t>NNP NNP VB NN JJ Z JJ Z VB Z UH Z CC WH SC VB NN NN SC JJ Z</t>
+  </si>
+  <si>
+    <t>IN NNP NNP Z SC VB WH RP IN NN FW FW FW IN NN PR Z</t>
+  </si>
+  <si>
+    <t>DT NN IN WH RP CC WH RP NN MD NN OD IN NN PR Z</t>
+  </si>
+  <si>
+    <t>NN NN VB NN X OD MD VB NN NNP IN NN CC NNP IN NNP Z</t>
+  </si>
+  <si>
+    <t>CD NND NN VB NN JJ IN NN CC NN SC VB NN NN Z</t>
+  </si>
+  <si>
+    <t>NN RB JJ NNP SC VB NN PR VB DT NN Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NNP PR RB VB IN NNP Z SC X IN NNP NEG JJ SC NN RP Z </t>
   </si>
 </sst>
 </file>
@@ -142,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,8 +200,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -251,26 +290,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -290,11 +309,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -323,43 +355,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -678,14 +698,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CD14569-BAA4-4BB5-9D07-C84D0FF9988D}">
   <dimension ref="B1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="88" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="92.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -695,17 +715,17 @@
         <v>0</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="17">
+      <c r="B2" s="13">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -714,9 +734,9 @@
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="18"/>
-      <c r="C3" s="11" t="s">
-        <v>15</v>
+      <c r="B3" s="14"/>
+      <c r="C3" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>2</v>
@@ -724,9 +744,9 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="18"/>
-      <c r="C4" s="12" t="s">
-        <v>16</v>
+      <c r="B4" s="14"/>
+      <c r="C4" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
@@ -734,462 +754,493 @@
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="18"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="2"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>31</v>
+      </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="18"/>
-      <c r="C6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="2"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="19"/>
-      <c r="C7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="2"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="20">
+      <c r="B8" s="13">
         <v>2</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="21"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="21"/>
-      <c r="C10" s="7" t="s">
-        <v>17</v>
+      <c r="B10" s="14"/>
+      <c r="C10" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="21"/>
-      <c r="C11" s="15"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="21"/>
-      <c r="C12" s="15"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="22"/>
-      <c r="C13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="20">
+      <c r="B14" s="13">
         <v>3</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="21"/>
-      <c r="C15" s="16"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="11"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="21"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="21"/>
-      <c r="C17" s="7" t="s">
-        <v>18</v>
+      <c r="B17" s="14"/>
+      <c r="C17" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="21"/>
-      <c r="C18" s="15"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="16" t="s">
+        <v>17</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="21"/>
-      <c r="C19" s="15"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="10"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="22"/>
-      <c r="C20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="7"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="20">
+      <c r="B21" s="13">
         <v>4</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>7</v>
+      <c r="C21" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="21"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="21"/>
-      <c r="C23" s="7" t="s">
-        <v>19</v>
+      <c r="B23" s="14"/>
+      <c r="C23" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="21"/>
-      <c r="C24" s="15"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="21"/>
-      <c r="C25" s="15"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="10"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="22"/>
-      <c r="C26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="7"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="20">
+      <c r="B27" s="13">
         <v>5</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>8</v>
+      <c r="C27" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="21"/>
+      <c r="B28" s="14"/>
       <c r="C28" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="21"/>
-      <c r="C29" s="7" t="s">
-        <v>20</v>
+      <c r="B29" s="14"/>
+      <c r="C29" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B30" s="21"/>
-      <c r="C30" s="15"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="16" t="s">
+        <v>35</v>
+      </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="21"/>
-      <c r="C31" s="15"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="10"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="22"/>
-      <c r="C32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="7"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="20">
+      <c r="B33" s="13">
         <v>6</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>9</v>
+      <c r="C33" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="21"/>
+      <c r="B34" s="14"/>
       <c r="C34" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="21"/>
-      <c r="C35" s="7" t="s">
-        <v>21</v>
+      <c r="B35" s="14"/>
+      <c r="C35" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="21"/>
-      <c r="C36" s="15"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="16" t="s">
+        <v>36</v>
+      </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B37" s="21"/>
-      <c r="C37" s="15"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="10"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B38" s="22"/>
-      <c r="C38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="7"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B39" s="20">
+      <c r="B39" s="13">
         <v>7</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>10</v>
+      <c r="C39" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B40" s="21"/>
+      <c r="B40" s="14"/>
       <c r="C40" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B41" s="21"/>
-      <c r="C41" s="7" t="s">
-        <v>22</v>
+      <c r="B41" s="14"/>
+      <c r="C41" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B42" s="21"/>
-      <c r="C42" s="15"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="16" t="s">
+        <v>37</v>
+      </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B43" s="21"/>
-      <c r="C43" s="15"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="10"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B44" s="22"/>
-      <c r="C44" s="15"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="7"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B45" s="20">
+      <c r="B45" s="13">
         <v>8</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>11</v>
+      <c r="C45" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B46" s="21"/>
+      <c r="B46" s="14"/>
       <c r="C46" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B47" s="21"/>
-      <c r="C47" s="7" t="s">
-        <v>23</v>
+      <c r="B47" s="14"/>
+      <c r="C47" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B48" s="21"/>
-      <c r="C48" s="15"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="16" t="s">
+        <v>38</v>
+      </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B49" s="21"/>
-      <c r="C49" s="15"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="10"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B50" s="22"/>
-      <c r="C50" s="15"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="7"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B51" s="20">
+      <c r="B51" s="13">
         <v>9</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>12</v>
+      <c r="C51" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B52" s="21"/>
+      <c r="B52" s="14"/>
       <c r="C52" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B53" s="21"/>
-      <c r="C53" s="7" t="s">
-        <v>24</v>
+      <c r="B53" s="14"/>
+      <c r="C53" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B54" s="21"/>
-      <c r="C54" s="15"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="16" t="s">
+        <v>39</v>
+      </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B55" s="21"/>
-      <c r="C55" s="15"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="10"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B56" s="22"/>
-      <c r="C56" s="15"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="7"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B57" s="20">
+      <c r="B57" s="13">
         <v>10</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>13</v>
+      <c r="C57" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B58" s="21"/>
+      <c r="B58" s="14"/>
       <c r="C58" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B59" s="21"/>
-      <c r="C59" s="7" t="s">
-        <v>25</v>
+      <c r="B59" s="14"/>
+      <c r="C59" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B60" s="21"/>
-      <c r="C60" s="15"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="16" t="s">
+        <v>40</v>
+      </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B61" s="21"/>
-      <c r="C61" s="15"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="10"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B62" s="22"/>
-      <c r="C62" s="15"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="7"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B63" s="13">
+      <c r="B63" s="12">
         <v>11</v>
       </c>
-      <c r="C63" s="10" t="s">
-        <v>14</v>
+      <c r="C63" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B64" s="13"/>
-      <c r="C64" s="11" t="s">
-        <v>15</v>
+      <c r="B64" s="12"/>
+      <c r="C64" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B65" s="13"/>
-      <c r="C65" s="12" t="s">
-        <v>26</v>
+      <c r="B65" s="18"/>
+      <c r="C65" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B66" s="13"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B67" s="13"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="10"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B68" s="13"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="B21:B26"/>
     <mergeCell ref="B57:B62"/>
     <mergeCell ref="B63:B68"/>
     <mergeCell ref="B27:B32"/>
@@ -1197,10 +1248,6 @@
     <mergeCell ref="B39:B44"/>
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="B51:B56"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="B14:B20"/>
-    <mergeCell ref="B21:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>